<commit_message>
Fixed tsv writing bug and updated samples.
</commit_message>
<xml_diff>
--- a/tests/sample_files/entity_dictionaries/bar__mapping.xlsx
+++ b/tests/sample_files/entity_dictionaries/bar__mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4950" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>authority</t>
   </si>
@@ -36,28 +36,19 @@
     <t>case_sensitive</t>
   </si>
   <si>
-    <t>tomes.test</t>
-  </si>
-  <si>
-    <t>bar {123} baz</t>
-  </si>
-  <si>
-    <t>bar {abc} baz</t>
-  </si>
-  <si>
-    <t>bar {abc123}</t>
-  </si>
-  <si>
-    <t>bar.123</t>
-  </si>
-  <si>
-    <t>bar.abc</t>
-  </si>
-  <si>
-    <t>bar.abc123</t>
-  </si>
-  <si>
     <t>Lorem ...</t>
+  </si>
+  <si>
+    <t>[0-9]{3}-[0-9]{2}-[0-9]{4}</t>
+  </si>
+  <si>
+    <t>PII.social_security_number</t>
+  </si>
+  <si>
+    <t>[0-9]{3} [0-9]{2} [0-9]{4}</t>
+  </si>
+  <si>
+    <t>bar_</t>
   </si>
 </sst>
 </file>
@@ -384,18 +375,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -418,50 +409,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>